<commit_message>
Update value remapping files which includes Power Query code
</commit_message>
<xml_diff>
--- a/Satellite launch overview/Excel files for value remapping/Remapping ucsusa to match n2yo.com dataset.xlsx
+++ b/Satellite launch overview/Excel files for value remapping/Remapping ucsusa to match n2yo.com dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Data Analysis\Dataset\Union of Concerned Scientists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Project\data-visualisation-datasets\Satellite launch overview\Excel files for value remapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32E07EF-5279-4897-8016-631CF5921F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAF3E76-FE64-4A99-A54C-B26FC8FE2CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="2325" windowWidth="16620" windowHeight="10500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3525" yWindow="2550" windowWidth="16320" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remap NORAD and COSPAR" sheetId="2" r:id="rId1"/>
@@ -1484,9 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CF4836-4D91-4C5F-84E4-1F95182401FC}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3501,7 +3499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D25235A-1B52-42AE-A1E4-3365BA4206D9}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>